<commit_message>
criação de documentos com qr code pronta E CELULAS PREENCHIDAS
</commit_message>
<xml_diff>
--- a/Templates/FF_Base.xlsx
+++ b/Templates/FF_Base.xlsx
@@ -125,17 +125,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial NARROW"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -234,11 +234,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,35 +246,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,7 +299,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q41" activeCellId="0" sqref="A1:Q41"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1341,10 +1341,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q41"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1364,10 +1364,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q41"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>